<commit_message>
Update report Wage Ledger.
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/WageLedgerNewLayoutTemplate.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/WageLedgerNewLayoutTemplate.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="214">
   <si>
     <t>1 月</t>
   </si>
@@ -650,9 +650,6 @@
   </si>
   <si>
     <t>SexInfo</t>
-  </si>
-  <si>
-    <t>【日通システム株式会社】</t>
   </si>
   <si>
     <t>対象期間</t>
@@ -716,7 +713,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -756,162 +753,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -1017,8 +858,112 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="hair">
+      <right style="dotted">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -1029,44 +974,18 @@
     </border>
     <border>
       <left/>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
+      <right style="dotted">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1078,32 +997,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1111,61 +1014,73 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1479,11 +1394,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A4:M35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:A33"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1492,38 +1405,33 @@
     <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D4" s="53"/>
-      <c r="F4" s="33" t="s">
+      <c r="D4" s="20"/>
+      <c r="F4" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="J4" s="53" t="s">
+      <c r="J4" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="L4" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="19" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1575,137 +1483,137 @@
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="21" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="20"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="M9" s="21" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="M10" s="25" t="s">
+      <c r="M10" s="24" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1713,137 +1621,137 @@
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="M11" s="15" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="20"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="L14" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="M14" s="25" t="s">
+      <c r="M14" s="24" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1851,81 +1759,81 @@
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="K15" s="16" t="s">
+      <c r="K15" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="16" t="s">
+      <c r="L15" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="M15" s="17" t="s">
+      <c r="M15" s="13" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="L16" s="21" t="s">
+      <c r="L16" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="M16" s="25" t="s">
+      <c r="M16" s="24" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1933,96 +1841,96 @@
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="J17" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="K17" s="13" t="s">
+      <c r="K17" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="L17" s="13" t="s">
+      <c r="L17" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="15" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="20"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="L19" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="M19" s="8" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2052,367 +1960,367 @@
         <v>28</v>
       </c>
       <c r="G22"/>
-      <c r="H22" s="38" t="s">
+      <c r="H22" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="39"/>
-      <c r="J22" s="42" t="s">
+      <c r="I22" s="36"/>
+      <c r="J22" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="43"/>
-      <c r="L22" s="44" t="s">
+      <c r="K22" s="40"/>
+      <c r="L22" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="M22" s="44"/>
+      <c r="M22" s="48"/>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="21" t="s">
         <v>159</v>
       </c>
       <c r="G23"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="31" t="s">
+      <c r="H23" s="37"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K23" s="31" t="s">
+      <c r="K23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
     </row>
     <row r="24" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
       <c r="G24"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="28"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="13"/>
     </row>
     <row r="25" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="21" t="s">
         <v>172</v>
       </c>
       <c r="G25"/>
-      <c r="H25" s="45">
+      <c r="H25" s="49">
         <f>SUM(B9:M9,B25:F25)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="46"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="54">
+      <c r="I25" s="50"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="47">
         <f>SUM(H25:K25)</f>
         <v>0</v>
       </c>
-      <c r="M25" s="37"/>
+      <c r="M25" s="34"/>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="24" t="s">
         <v>176</v>
       </c>
       <c r="G26"/>
-      <c r="H26" s="47">
+      <c r="H26" s="41">
         <f>SUM(B10:M10,B26:F26)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="48"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="28"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="13"/>
     </row>
     <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="15" t="s">
         <v>180</v>
       </c>
       <c r="G27"/>
-      <c r="H27" s="49">
+      <c r="H27" s="45">
         <f>SUM(B11:M11,B27:F27)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="50"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="28"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="13"/>
     </row>
     <row r="28" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="20"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="8"/>
       <c r="G28"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="28"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="13"/>
     </row>
     <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="26" t="s">
         <v>181</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="G29" s="22"/>
-      <c r="H29" s="45">
+      <c r="G29" s="9"/>
+      <c r="H29" s="49">
         <f>SUM(B13:M13,B29:F29)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="46"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="37"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="34"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="F30" s="25" t="s">
+      <c r="F30" s="24" t="s">
         <v>188</v>
       </c>
       <c r="G30"/>
-      <c r="H30" s="47">
+      <c r="H30" s="41">
         <f>SUM(B14:M14,B30:F30)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="48"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="28"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="13"/>
     </row>
     <row r="31" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="13" t="s">
         <v>192</v>
       </c>
       <c r="G31"/>
-      <c r="H31" s="51">
+      <c r="H31" s="43">
         <f>SUM(B15:M15,B31:F31)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="52"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="37"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="34"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="F32" s="25" t="s">
+      <c r="F32" s="24" t="s">
         <v>196</v>
       </c>
       <c r="G32"/>
-      <c r="H32" s="47">
+      <c r="H32" s="41">
         <f>SUM(B16:M16,B32:F32)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="48"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-      <c r="L32" s="27"/>
-      <c r="M32" s="28"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="13"/>
     </row>
     <row r="33" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="15" t="s">
         <v>200</v>
       </c>
       <c r="G33"/>
-      <c r="H33" s="49">
+      <c r="H33" s="45">
         <f>SUM(B17:M17,B33:F33)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="50"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="28"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="13"/>
     </row>
     <row r="34" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="20"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
       <c r="G34"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="28"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="13"/>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="8" t="s">
         <v>204</v>
       </c>
       <c r="G35"/>
-      <c r="H35" s="36">
+      <c r="H35" s="33">
         <f>SUM(B19:M19,B35:F35)</f>
         <v>0</v>
       </c>
-      <c r="I35" s="37"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="30"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2432,7 +2340,11 @@
     <mergeCell ref="H32:I32"/>
     <mergeCell ref="H33:I33"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="62" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;L&amp;13【日通システム株式会社】 </oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Entity For Query Data Report QET001.
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/WageLedgerNewLayoutTemplate.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/WageLedgerNewLayoutTemplate.xlsx
@@ -665,6 +665,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0;\-#,##0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -985,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1017,22 +1020,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1053,34 +1047,50 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1483,40 +1493,40 @@
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="32" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1539,40 +1549,40 @@
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="L9" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="M9" s="32" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1580,40 +1590,40 @@
       <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="K10" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="L10" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="M10" s="37" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1621,40 +1631,40 @@
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="K11" s="30" t="s">
+      <c r="K11" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="40" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1677,40 +1687,40 @@
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K13" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="L13" s="26" t="s">
+      <c r="L13" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="M13" s="32" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1718,40 +1728,40 @@
       <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="K14" s="28" t="s">
+      <c r="K14" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="L14" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="M14" s="24" t="s">
+      <c r="M14" s="37" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1759,40 +1769,40 @@
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="32" t="s">
+      <c r="H15" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="I15" s="32" t="s">
+      <c r="I15" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="32" t="s">
+      <c r="J15" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="K15" s="32" t="s">
+      <c r="K15" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="32" t="s">
+      <c r="L15" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="M15" s="13" t="s">
+      <c r="M15" s="43" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1800,40 +1810,40 @@
       <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="J16" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="K16" s="28" t="s">
+      <c r="K16" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="L16" s="28" t="s">
+      <c r="L16" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="M16" s="24" t="s">
+      <c r="M16" s="37" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1841,40 +1851,40 @@
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="H17" s="30" t="s">
+      <c r="H17" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="I17" s="30" t="s">
+      <c r="I17" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="J17" s="30" t="s">
+      <c r="J17" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="K17" s="30" t="s">
+      <c r="K17" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="L17" s="30" t="s">
+      <c r="L17" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="M17" s="15" t="s">
+      <c r="M17" s="40" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1897,40 +1907,40 @@
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="K19" s="23" t="s">
+      <c r="K19" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="M19" s="44" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1960,57 +1970,57 @@
         <v>28</v>
       </c>
       <c r="G22"/>
-      <c r="H22" s="35" t="s">
+      <c r="H22" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I22" s="36"/>
-      <c r="J22" s="39" t="s">
+      <c r="I22" s="25"/>
+      <c r="J22" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="K22" s="40"/>
-      <c r="L22" s="48" t="s">
+      <c r="K22" s="29"/>
+      <c r="L22" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="M22" s="48"/>
+      <c r="M22" s="22"/>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="32" t="s">
         <v>159</v>
       </c>
       <c r="G23"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="38"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
       <c r="J23" s="16" t="s">
         <v>32</v>
       </c>
       <c r="K23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="L23" s="48"/>
-      <c r="M23" s="48"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="44"/>
       <c r="G24"/>
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
@@ -2023,60 +2033,60 @@
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="32" t="s">
         <v>172</v>
       </c>
       <c r="G25"/>
-      <c r="H25" s="49">
+      <c r="H25" s="46">
         <f>SUM(B9:M9,B25:F25)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="50"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="47">
+      <c r="I25" s="47"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="48">
         <f>SUM(H25:K25)</f>
         <v>0</v>
       </c>
-      <c r="M25" s="34"/>
+      <c r="M25" s="49"/>
     </row>
     <row r="26" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="37" t="s">
         <v>176</v>
       </c>
       <c r="G26"/>
-      <c r="H26" s="41">
+      <c r="H26" s="50">
         <f>SUM(B10:M10,B26:F26)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="42"/>
+      <c r="I26" s="51"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
@@ -2086,27 +2096,27 @@
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="40" t="s">
         <v>180</v>
       </c>
       <c r="G27"/>
-      <c r="H27" s="45">
+      <c r="H27" s="52">
         <f>SUM(B11:M11,B27:F27)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="46"/>
+      <c r="I27" s="53"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
@@ -2114,11 +2124,11 @@
     </row>
     <row r="28" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="8"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="44"/>
       <c r="G28"/>
       <c r="H28" s="11"/>
       <c r="I28" s="12"/>
@@ -2131,57 +2141,57 @@
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="F29" s="32" t="s">
         <v>184</v>
       </c>
       <c r="G29" s="9"/>
-      <c r="H29" s="49">
+      <c r="H29" s="46">
         <f>SUM(B13:M13,B29:F29)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="50"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="34"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="49"/>
     </row>
     <row r="30" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E30" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="F30" s="37" t="s">
         <v>188</v>
       </c>
       <c r="G30"/>
-      <c r="H30" s="41">
+      <c r="H30" s="50">
         <f>SUM(B14:M14,B30:F30)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="42"/>
+      <c r="I30" s="51"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
@@ -2191,57 +2201,57 @@
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="41" t="s">
         <v>165</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="43" t="s">
         <v>192</v>
       </c>
       <c r="G31"/>
-      <c r="H31" s="43">
+      <c r="H31" s="54">
         <f>SUM(B15:M15,B31:F31)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="44"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="34"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="49"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="F32" s="37" t="s">
         <v>196</v>
       </c>
       <c r="G32"/>
-      <c r="H32" s="41">
+      <c r="H32" s="50">
         <f>SUM(B16:M16,B32:F32)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="42"/>
+      <c r="I32" s="51"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
@@ -2251,27 +2261,27 @@
       <c r="A33" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="E33" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="40" t="s">
         <v>200</v>
       </c>
       <c r="G33"/>
-      <c r="H33" s="45">
+      <c r="H33" s="52">
         <f>SUM(B17:M17,B33:F33)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="46"/>
+      <c r="I33" s="53"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
@@ -2279,11 +2289,11 @@
     </row>
     <row r="34" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="44"/>
       <c r="G34"/>
       <c r="H34" s="11"/>
       <c r="I34" s="12"/>
@@ -2296,27 +2306,27 @@
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="44" t="s">
         <v>204</v>
       </c>
       <c r="G35"/>
-      <c r="H35" s="33">
+      <c r="H35" s="23">
         <f>SUM(B19:M19,B35:F35)</f>
         <v>0</v>
       </c>
-      <c r="I35" s="34"/>
+      <c r="I35" s="21"/>
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
       <c r="L35" s="14"/>
@@ -2324,6 +2334,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H22:I23"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
     <mergeCell ref="L31:M31"/>
     <mergeCell ref="L22:M23"/>
     <mergeCell ref="H25:I25"/>
@@ -2332,13 +2349,6 @@
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="L25:M25"/>
     <mergeCell ref="L29:M29"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H22:I23"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>